<commit_message>
Updated code with loading details method and new xpath of latest Build
# Conflicts:
#	Test Data/TC_135_Verify_Isolator_Units_Calculation_With_Loop_Having_Line_Isolator_Devices.xlsx
</commit_message>
<xml_diff>
--- a/Test Data/TC_114_Verify_Cable_capacitance.xlsx
+++ b/Test Data/TC_114_Verify_Cable_capacitance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdhakaa\Documents\NG Consys Project\Testing\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6190EDC-6A19-4B95-8A1A-F9AC3FD011E2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29317B7E-C62C-4287-B352-C7D3AC7D4631}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Devices" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="25">
   <si>
     <t>Devices</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>To verify cable capacitance</t>
+  </si>
+  <si>
+    <t>AC Loading Details Name</t>
+  </si>
+  <si>
+    <t>Signal (AC Units)</t>
   </si>
 </sst>
 </file>
@@ -485,7 +491,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,7 +513,9 @@
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -521,6 +529,9 @@
         <v>14</v>
       </c>
       <c r="D2" s="12"/>
+      <c r="G2" s="7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">

</xml_diff>

<commit_message>
Updated test data for cable capacitance and other test cases
</commit_message>
<xml_diff>
--- a/Test Data/TC_114_Verify_Cable_capacitance.xlsx
+++ b/Test Data/TC_114_Verify_Cable_capacitance.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29317B7E-C62C-4287-B352-C7D3AC7D4631}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Devices" sheetId="1" r:id="rId1"/>
@@ -106,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,11 +486,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -609,10 +608,10 @@
         <v>6</v>
       </c>
       <c r="G8" s="8">
-        <v>20.399989999999999</v>
+        <v>20</v>
       </c>
       <c r="H8" s="8">
-        <v>171.6</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -635,10 +634,10 @@
         <v>6</v>
       </c>
       <c r="G9" s="8">
-        <v>55.599989999999998</v>
+        <v>56</v>
       </c>
       <c r="H9" s="8">
-        <v>152.80000000000001</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -678,7 +677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5D2B0D-FC00-40D5-BB84-8C7D3159CE3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">

</xml_diff>